<commit_message>
-Updated the WP Budget
Former-commit-id: c79c1c3e07bb709ba961703ec20a7a69b303ac9f
</commit_message>
<xml_diff>
--- a/data/AGE-WELL WP Budget.xlsx
+++ b/data/AGE-WELL WP Budget.xlsx
@@ -16,6 +16,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Overall Project Budget'!$A$1:$M$29</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Overall Project Budget'!$A$1:$M$29</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Overall Project Budget'!$A$1:$M$29</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Overall Project Budget'!$A$1:$M$29</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -42,7 +43,7 @@
     <t>Names of Investigators Receiving Funding</t>
   </si>
   <si>
-    <t>April 1, 2016 - March 31, 2017</t>
+    <t>April 1, 2017 - March 31, 2018</t>
   </si>
   <si>
     <t>Expenditure Categories</t>
@@ -556,7 +557,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Excel Built-in Excel Built-in Normal 2" xfId="20" builtinId="54" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -630,7 +631,7 @@
   <dimension ref="1:26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>

</xml_diff>